<commit_message>
Updated comment and test data sheet.
</commit_message>
<xml_diff>
--- a/Data/TESTSUITE1.xlsx
+++ b/Data/TESTSUITE1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\370313\Documents\ZohotTesting\ZohoTesting\DataDriven_Framework\Datadriven_Framework_MVN\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Airline_Hybrid_MVN\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>st</t>
-  </si>
-  <si>
-    <t>prod</t>
   </si>
   <si>
     <t>browser</t>
@@ -734,7 +731,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +757,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,10 +768,10 @@
         <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,7 +785,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating all the changes.
</commit_message>
<xml_diff>
--- a/Data/TESTSUITE1.xlsx
+++ b/Data/TESTSUITE1.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\Airline_Hybrid_MVN\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23730" windowHeight="8865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12975" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FlightResults" sheetId="2" r:id="rId1"/>
     <sheet name="FlightData" sheetId="3" r:id="rId2"/>
     <sheet name="Keywords" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
   <si>
     <t>TCID</t>
   </si>
@@ -82,12 +78,6 @@
     <t>ATL</t>
   </si>
   <si>
-    <t>2/1/2017</t>
-  </si>
-  <si>
-    <t>2/6/2017</t>
-  </si>
-  <si>
     <t>Flight#</t>
   </si>
   <si>
@@ -155,6 +145,24 @@
   </si>
   <si>
     <t>Mozilla</t>
+  </si>
+  <si>
+    <t>readResultsTable</t>
+  </si>
+  <si>
+    <t>resultTable_xpath</t>
+  </si>
+  <si>
+    <t>3/30/2017</t>
+  </si>
+  <si>
+    <t>4/10/2017</t>
+  </si>
+  <si>
+    <t>3/1/2017</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -657,7 +665,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -731,7 +739,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -765,27 +773,27 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -796,10 +804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -830,7 +838,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -841,7 +849,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -852,7 +860,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -865,7 +873,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -880,7 +888,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -893,7 +901,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
@@ -903,12 +911,12 @@
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -921,7 +929,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
@@ -931,25 +939,25 @@
         <v>13</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -962,7 +970,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -972,40 +980,40 @@
         <v>14</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -1018,215 +1026,228 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>33</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D21" s="34"/>
       <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E22" s="34"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>17</v>
-      </c>
+      <c r="E23" s="34"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="35"/>
+        <v>11</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="34"/>
-      <c r="C25" s="33" t="s">
-        <v>9</v>
+      <c r="C25" s="34" t="s">
+        <v>8</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="34" t="s">
-        <v>21</v>
-      </c>
+      <c r="E25" s="35"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="34"/>
-      <c r="C26" s="34" t="s">
-        <v>8</v>
+      <c r="C26" s="33" t="s">
+        <v>9</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="34"/>
+        <v>12</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="36"/>
+        <v>30</v>
+      </c>
+      <c r="B27" s="34"/>
       <c r="C27" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="33"/>
+        <v>21</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="33"/>
+      <c r="E32" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>